<commit_message>
testing and simulation setups
</commit_message>
<xml_diff>
--- a/Documents/Timeline_2025.xlsx
+++ b/Documents/Timeline_2025.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC1048FA699B42E05ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA385A41-D8D5-4F3A-8317-75F20E7CA0D3}"/>
   <bookViews>
-    <workbookView xWindow="5856" yWindow="3636" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>